<commit_message>
Tested most workflows up to adding action data, fixed bugs
</commit_message>
<xml_diff>
--- a/TestSpreadsheet.xlsx
+++ b/TestSpreadsheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Full name</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>test9</t>
+  </si>
+  <si>
+    <t>Service Code</t>
+  </si>
+  <si>
+    <t>RSD</t>
   </si>
 </sst>
 </file>
@@ -59,7 +65,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -106,7 +112,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -408,7 +414,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -437,7 +443,9 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
@@ -458,7 +466,9 @@
       <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
added service / data for testing
</commit_message>
<xml_diff>
--- a/TestSpreadsheet.xlsx
+++ b/TestSpreadsheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Full name</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>RSD</t>
+  </si>
+  <si>
+    <t>Action Name</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -411,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -424,7 +430,7 @@
     <col min="3" max="1024" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25.5">
+    <row r="1" spans="1:8" ht="25.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -446,8 +452,11 @@
       <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -468,6 +477,9 @@
       </c>
       <c r="G2" s="3" t="s">
         <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished CtrlAddAction code (needs to be tested)
</commit_message>
<xml_diff>
--- a/TestSpreadsheet.xlsx
+++ b/TestSpreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7515" windowHeight="7560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Full name</t>
   </si>
@@ -64,6 +64,18 @@
   </si>
   <si>
     <t>Other</t>
+  </si>
+  <si>
+    <t>Action caseworker</t>
+  </si>
+  <si>
+    <t>Attendance Notes</t>
+  </si>
+  <si>
+    <t>abeaman</t>
+  </si>
+  <si>
+    <t>notes</t>
   </si>
 </sst>
 </file>
@@ -417,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -430,7 +442,7 @@
     <col min="3" max="1024" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="25.5">
+    <row r="1" spans="1:10" ht="25.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,8 +467,14 @@
       <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -480,6 +498,12 @@
       </c>
       <c r="H2" t="s">
         <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished most controllers, fixed up field translators, tested a few workflows
</commit_message>
<xml_diff>
--- a/TestSpreadsheet.xlsx
+++ b/TestSpreadsheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
   <si>
     <t>Full name</t>
   </si>
@@ -36,21 +36,12 @@
     <t>Phone NUMBer</t>
   </si>
   <si>
-    <t>UNHCR no</t>
-  </si>
-  <si>
     <t>Alex Test6</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
     <t>.10/28/2010</t>
   </si>
   <si>
-    <t>Sudanese</t>
-  </si>
-  <si>
     <t>test9</t>
   </si>
   <si>
@@ -76,6 +67,57 @@
   </si>
   <si>
     <t>notes</t>
+  </si>
+  <si>
+    <t>Main Language</t>
+  </si>
+  <si>
+    <t>Arabic</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>UNHCR nUMber</t>
+  </si>
+  <si>
+    <t>Sudan</t>
+  </si>
+  <si>
+    <t>TEST SCENARIO #99</t>
+  </si>
+  <si>
+    <t>TEST SCENARIO #6</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>UNHCR Number</t>
+  </si>
+  <si>
+    <t>TEST SCENARIO #7</t>
+  </si>
+  <si>
+    <t>Service Caseworker</t>
+  </si>
+  <si>
+    <t>AFP</t>
+  </si>
+  <si>
+    <t>Client Appointment</t>
+  </si>
+  <si>
+    <t>Action Caseworker</t>
+  </si>
+  <si>
+    <t>Action notes</t>
+  </si>
+  <si>
+    <t>woot!!</t>
   </si>
 </sst>
 </file>
@@ -85,7 +127,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -93,13 +135,21 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -121,19 +171,25 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -429,86 +485,259 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A5:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" customWidth="1"/>
-    <col min="3" max="1024" width="11.5703125"/>
+    <col min="1" max="1" width="20.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="11.5703125" style="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="1025" width="11.5703125" style="1"/>
+    <col min="1026" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5">
-      <c r="A1" s="1" t="s">
+    <row r="5" spans="1:12">
+      <c r="A5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1234567890</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1234567890</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:12" ht="25.5">
+      <c r="A14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1234567890</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1234567890</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A9:C9"/>
+  </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
Moving data input / results to options page, not popup.
</commit_message>
<xml_diff>
--- a/TestSpreadsheet.xlsx
+++ b/TestSpreadsheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="37">
   <si>
     <t>Full name</t>
   </si>
@@ -118,6 +118,18 @@
   </si>
   <si>
     <t>woot!!</t>
+  </si>
+  <si>
+    <t>Alex Correct Format</t>
+  </si>
+  <si>
+    <t>.10/25/2003</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>1111/2222</t>
   </si>
 </sst>
 </file>
@@ -485,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A5:L15"/>
+  <dimension ref="A5:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="A6" sqref="A6:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -538,16 +550,16 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>20</v>
@@ -556,185 +568,211 @@
         <v>1234567890</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="5" t="s">
+    <row r="8" spans="1:12">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1234567890</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:12">
+      <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F12" s="2">
         <v>1234567890</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="5" t="s">
+    <row r="14" spans="1:12">
+      <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="1:12" ht="25.5">
-      <c r="A14" s="2" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:12" ht="25.5">
+      <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="2" t="s">
+    <row r="16" spans="1:12">
+      <c r="A16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F16" s="2">
         <v>1234567890</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
     <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Big push - v0.2.0 - Very close to being ready for Phase 1
</commit_message>
<xml_diff>
--- a/TestSpreadsheet.xlsx
+++ b/TestSpreadsheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="50">
   <si>
     <t>Full name</t>
   </si>
@@ -123,21 +123,61 @@
     <t>Alex Correct Format</t>
   </si>
   <si>
-    <t>.10/25/2003</t>
-  </si>
-  <si>
     <t>English</t>
   </si>
   <si>
     <t>1111/2222</t>
+  </si>
+  <si>
+    <t>555-55C55555</t>
+  </si>
+  <si>
+    <t>.09/10/2003</t>
+  </si>
+  <si>
+    <t>TEST SCENARIO #0</t>
+  </si>
+  <si>
+    <t>UNHCR Status</t>
+  </si>
+  <si>
+    <t>Blue Card</t>
+  </si>
+  <si>
+    <t>White Paper</t>
+  </si>
+  <si>
+    <t>1111/3333</t>
+  </si>
+  <si>
+    <t>Service Start Date</t>
+  </si>
+  <si>
+    <t>UNHCR Case Size</t>
+  </si>
+  <si>
+    <t>Alex2 Correct Format2</t>
+  </si>
+  <si>
+    <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>.09/13/2003</t>
+  </si>
+  <si>
+    <t>30/5/2017</t>
+  </si>
+  <si>
+    <t>MED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -187,7 +227,7 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -198,6 +238,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -497,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A5:L16"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:H7"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -510,82 +553,172 @@
     <col min="3" max="3" width="11.5703125" style="1"/>
     <col min="4" max="4" width="9.140625" style="1"/>
     <col min="5" max="5" width="11.5703125" style="1"/>
-    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="1025" width="11.5703125" style="1"/>
+    <col min="6" max="6" width="13.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="1025" width="11.5703125" style="1"/>
     <col min="1026" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:12">
-      <c r="A5" s="5" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1234567890</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="5">
+        <v>42738</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1234567890</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="1">
+        <v>3</v>
+      </c>
+      <c r="J4" s="5">
+        <v>38444</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1234567890</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="2" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>20</v>
@@ -594,185 +727,220 @@
         <v>1234567890</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="5" t="s">
+    <row r="9" spans="1:12">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1234567890</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:12">
+      <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F13" s="2">
         <v>1234567890</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="5" t="s">
+    <row r="18" spans="1:11">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-    </row>
-    <row r="15" spans="1:12" ht="25.5">
-      <c r="A15" s="2" t="s">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+    </row>
+    <row r="20" spans="1:11" ht="25.5">
+      <c r="A20" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J20" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K20" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="2" t="s">
+    <row r="21" spans="1:11">
+      <c r="A21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F21" s="2">
         <v>1234567890</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A10:C10"/>
+  <mergeCells count="4">
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added functionality for 2 languages in 'Main Language' column.
</commit_message>
<xml_diff>
--- a/TestSpreadsheet.xlsx
+++ b/TestSpreadsheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="52">
   <si>
     <t>Full name</t>
   </si>
@@ -162,13 +162,19 @@
     <t>Ethiopia</t>
   </si>
   <si>
-    <t>.09/13/2003</t>
-  </si>
-  <si>
     <t>30/5/2017</t>
   </si>
   <si>
     <t>MED</t>
+  </si>
+  <si>
+    <t>Arabic,Fir</t>
+  </si>
+  <si>
+    <t>.09/12/2003</t>
+  </si>
+  <si>
+    <t>English, Bilen, Arabic</t>
   </si>
 </sst>
 </file>
@@ -204,12 +210,18 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -227,7 +239,7 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -244,6 +256,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -540,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -551,7 +566,7 @@
     <col min="1" max="1" width="20.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="6.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" style="1"/>
-    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="4" max="4" width="15.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" style="1"/>
     <col min="6" max="6" width="13.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.140625" style="1" customWidth="1"/>
@@ -604,7 +619,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" ht="25.5">
       <c r="A3" s="2" t="s">
         <v>33</v>
       </c>
@@ -612,10 +627,10 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>46</v>
@@ -630,13 +645,13 @@
         <v>40</v>
       </c>
       <c r="I3" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="J3" s="5">
         <v>42738</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -647,10 +662,10 @@
         <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>17</v>
+        <v>47</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>20</v>
@@ -674,77 +689,60 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="6" t="s">
+    <row r="5" spans="1:12">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1234567890</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>20</v>
@@ -753,193 +751,219 @@
         <v>1234567890</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="6" t="s">
+    <row r="10" spans="1:12">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1234567890</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:12">
+      <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F14" s="2">
         <v>1234567890</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-    </row>
-    <row r="20" spans="1:11" ht="25.5">
-      <c r="A20" s="2" t="s">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="1:11" ht="25.5">
+      <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="I21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="J21" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="K21" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="2" t="s">
+    <row r="22" spans="1:11">
+      <c r="A22" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F22" s="2">
         <v>1234567890</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="I22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A12:C12"/>
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
Fixed #6 - CBI saving error
</commit_message>
<xml_diff>
--- a/TestSpreadsheet.xlsx
+++ b/TestSpreadsheet.xlsx
@@ -557,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -645,7 +645,7 @@
         <v>40</v>
       </c>
       <c r="I3" s="1">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="J3" s="5">
         <v>42738</v>

</xml_diff>

<commit_message>
Now skips client when fatal error found on Registration page by RIPS validation extension
</commit_message>
<xml_diff>
--- a/TestSpreadsheet.xlsx
+++ b/TestSpreadsheet.xlsx
@@ -239,7 +239,7 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -258,6 +258,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -558,7 +561,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -635,8 +638,8 @@
       <c r="E3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="2">
-        <v>1234567890</v>
+      <c r="F3" s="8">
+        <v>555</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
New spreadsheet tests, new screenshots for published extension
</commit_message>
<xml_diff>
--- a/TestSpreadsheet.xlsx
+++ b/TestSpreadsheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
   <si>
     <t>Full name</t>
   </si>
@@ -156,9 +156,6 @@
     <t>UNHCR Case Size</t>
   </si>
   <si>
-    <t>Alex2 Correct Format2</t>
-  </si>
-  <si>
     <t>Ethiopia</t>
   </si>
   <si>
@@ -168,13 +165,31 @@
     <t>MED</t>
   </si>
   <si>
-    <t>Arabic,Fir</t>
-  </si>
-  <si>
     <t>.09/12/2003</t>
   </si>
   <si>
     <t>English, Bilen, Arabic</t>
+  </si>
+  <si>
+    <t>Mister Correct Format</t>
+  </si>
+  <si>
+    <t>Test Correct Format2</t>
+  </si>
+  <si>
+    <t>Arabic,Fur</t>
+  </si>
+  <si>
+    <t>Jane Doe</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Yemen</t>
+  </si>
+  <si>
+    <t>1111/4444</t>
   </si>
 </sst>
 </file>
@@ -210,18 +225,12 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -257,10 +266,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -558,16 +567,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K4"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="20.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" style="1"/>
     <col min="4" max="4" width="15.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" style="1"/>
@@ -624,22 +633,22 @@
     </row>
     <row r="3" spans="1:12" ht="25.5">
       <c r="A3" s="2" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F3" s="8">
-        <v>555</v>
+        <v>1111111111</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>35</v>
@@ -654,21 +663,21 @@
         <v>42738</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>20</v>
@@ -693,280 +702,322 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="5">
+        <v>8739</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="2">
+        <v>9999999999</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="J5" s="5"/>
     </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="J6" s="5"/>
+    </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="1" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="2" t="s">
+    <row r="12" spans="1:12">
+      <c r="A12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F12" s="2">
         <v>1234567890</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="2" t="s">
+    <row r="13" spans="1:12">
+      <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F13" s="2">
         <v>1234567890</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="6" t="s">
+    <row r="15" spans="1:12">
+      <c r="A15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="1" t="s">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="2" t="s">
+    <row r="17" spans="1:12">
+      <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F17" s="2">
         <v>1234567890</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="6" t="s">
+    <row r="22" spans="1:12">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-    </row>
-    <row r="21" spans="1:11" ht="25.5">
-      <c r="A21" s="2" t="s">
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+    </row>
+    <row r="24" spans="1:12" ht="25.5">
+      <c r="A24" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G24" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="I24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="J24" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="K24" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="2" t="s">
+    <row r="25" spans="1:12">
+      <c r="A25" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F25" s="2">
         <v>1234567890</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="K25" s="1" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A15:C15"/>
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
Edits made for publishing on web store
</commit_message>
<xml_diff>
--- a/TestSpreadsheet.xlsx
+++ b/TestSpreadsheet.xlsx
@@ -263,14 +263,14 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -570,19 +570,19 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="20.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="1"/>
+    <col min="3" max="3" width="11.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="1"/>
+    <col min="5" max="5" width="11.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="14.140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="1025" width="11.5703125" style="1"/>
@@ -590,11 +590,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
@@ -647,7 +647,7 @@
       <c r="E3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>1111111111</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -676,7 +676,7 @@
       <c r="C4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>52</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -711,7 +711,7 @@
       <c r="C5" s="5">
         <v>8739</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -729,7 +729,7 @@
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="5"/>
-      <c r="D6" s="7"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="J6" s="5"/>
@@ -738,7 +738,7 @@
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="7"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="J7" s="5"/>
@@ -753,11 +753,11 @@
       <c r="J8" s="5"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
@@ -838,11 +838,11 @@
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="1" t="s">
@@ -929,11 +929,11 @@
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>

</xml_diff>

<commit_message>
slight test spreadsheet changes
</commit_message>
<xml_diff>
--- a/TestSpreadsheet.xlsx
+++ b/TestSpreadsheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="65">
   <si>
     <t>Full name</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Action notes</t>
   </si>
   <si>
-    <t>woot!!</t>
-  </si>
-  <si>
     <t>Alex Correct Format</t>
   </si>
   <si>
@@ -162,9 +159,6 @@
     <t>30/5/2017</t>
   </si>
   <si>
-    <t>MED</t>
-  </si>
-  <si>
     <t>.09/12/2003</t>
   </si>
   <si>
@@ -192,7 +186,34 @@
     <t>Bob Vans</t>
   </si>
   <si>
-    <t>1111/1122</t>
+    <t>1111/1111</t>
+  </si>
+  <si>
+    <t>OUT</t>
+  </si>
+  <si>
+    <t>Alejandro Jimmithy Burr</t>
+  </si>
+  <si>
+    <t>1111/1234</t>
+  </si>
+  <si>
+    <t>MAN</t>
+  </si>
+  <si>
+    <t>Aww giggidy, let's get some boxes!</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>Referred for food &amp; hygiene box</t>
+  </si>
+  <si>
+    <t>Oh snap! A note!</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -251,7 +272,7 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -275,6 +296,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -570,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -594,7 +616,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -622,13 +644,13 @@
         <v>25</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>8</v>
@@ -636,61 +658,63 @@
     </row>
     <row r="3" spans="1:12" ht="25.5">
       <c r="A3" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>48</v>
+      <c r="C3" s="5">
+        <v>8739</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" s="7"/>
+        <v>44</v>
+      </c>
+      <c r="F3" s="7">
+        <v>11234567890</v>
+      </c>
       <c r="G3" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J3" s="5">
         <v>42738</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F4" s="2">
-        <v>1234567890</v>
+        <v>11234567890</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I4" s="1">
         <v>3</v>
@@ -699,30 +723,30 @@
         <v>38444</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="5">
-        <v>8739</v>
+        <v>51</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F5" s="2">
         <v>9999999999</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J5" s="5"/>
     </row>
@@ -788,16 +812,16 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>20</v>
@@ -806,7 +830,7 @@
         <v>1234567890</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>9</v>
@@ -832,7 +856,7 @@
         <v>1234567890</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>9</v>
@@ -903,7 +927,7 @@
         <v>1234567890</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>28</v>
@@ -915,108 +939,146 @@
         <v>29</v>
       </c>
       <c r="K17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="25.5">
+      <c r="A18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="9">
+        <v>16593</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1234567890</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L17" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="L18" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="8" t="s">
+      <c r="A22" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-    </row>
-    <row r="24" spans="1:12" ht="25.5">
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+    </row>
+    <row r="23" spans="1:12" ht="25.5">
+      <c r="A23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F24" s="2">
         <v>1234567890</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A22:C22"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A1:C1"/>

</xml_diff>

<commit_message>
Moved client data 'get' to MainController
</commit_message>
<xml_diff>
--- a/TestSpreadsheet.xlsx
+++ b/TestSpreadsheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="96">
   <si>
     <t>Full name</t>
   </si>
@@ -192,15 +192,9 @@
     <t>OUT</t>
   </si>
   <si>
-    <t>Alejandro Jimmithy Burr</t>
-  </si>
-  <si>
     <t>1111/1234</t>
   </si>
   <si>
-    <t>MAN</t>
-  </si>
-  <si>
     <t>Aww giggidy, let's get some boxes!</t>
   </si>
   <si>
@@ -214,6 +208,105 @@
   </si>
   <si>
     <t>none</t>
+  </si>
+  <si>
+    <t>Unregistered</t>
+  </si>
+  <si>
+    <t>RST</t>
+  </si>
+  <si>
+    <t>Alejan TEST</t>
+  </si>
+  <si>
+    <t>NATIOnality</t>
+  </si>
+  <si>
+    <t>Alejandro Jimmitthy Burr</t>
+  </si>
+  <si>
+    <t>wee</t>
+  </si>
+  <si>
+    <t>Received clothes distribution</t>
+  </si>
+  <si>
+    <t>DA</t>
+  </si>
+  <si>
+    <t>Direct beneficiaries</t>
+  </si>
+  <si>
+    <t>TEST SCENARIO #8 (FROM DAP MASTER LIST)</t>
+  </si>
+  <si>
+    <t>UNHCR number</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Date Of Birth</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Exclution date</t>
+  </si>
+  <si>
+    <t>Location in Cairo (if known)</t>
+  </si>
+  <si>
+    <t>Telephone # 2</t>
+  </si>
+  <si>
+    <t>555-15C11941</t>
+  </si>
+  <si>
+    <t>17 yr, 9 mon</t>
+  </si>
+  <si>
+    <t>Eritria</t>
+  </si>
+  <si>
+    <t>Faisal</t>
+  </si>
+  <si>
+    <t>Tigrinya</t>
+  </si>
+  <si>
+    <t>555-00159404</t>
+  </si>
+  <si>
+    <t>9 yr, 6 mon</t>
+  </si>
+  <si>
+    <t>S.Sudan</t>
+  </si>
+  <si>
+    <t>Maadi</t>
+  </si>
+  <si>
+    <t>555-00191459</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>test135</t>
+  </si>
+  <si>
+    <t>test246</t>
+  </si>
+  <si>
+    <t>test357</t>
+  </si>
+  <si>
+    <t>alex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last name   </t>
   </si>
 </sst>
 </file>
@@ -272,7 +365,7 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -293,10 +386,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -592,36 +692,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B16" sqref="A16:O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="20.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="1025" width="11.5703125" style="1"/>
-    <col min="1026" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="25.5703125" style="1" customWidth="1"/>
+    <col min="14" max="1026" width="11.5703125" style="1"/>
+    <col min="1027" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:15">
+      <c r="A1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -649,14 +752,14 @@
       <c r="I2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="25.5">
+    <row r="3" spans="1:15" ht="25.5">
       <c r="A3" s="2" t="s">
         <v>48</v>
       </c>
@@ -684,14 +787,14 @@
       <c r="I3" s="1">
         <v>2</v>
       </c>
-      <c r="J3" s="5">
+      <c r="K3" s="5">
         <v>42738</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:15">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -719,14 +822,14 @@
       <c r="I4" s="1">
         <v>3</v>
       </c>
-      <c r="J4" s="5">
+      <c r="K4" s="5">
         <v>38444</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:15">
       <c r="A5" s="2" t="s">
         <v>54</v>
       </c>
@@ -748,43 +851,43 @@
       <c r="G5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="5"/>
       <c r="D6" s="6"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="5"/>
       <c r="D8" s="3"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="8" t="s">
+      <c r="K8" s="5"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -810,7 +913,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:15">
       <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
@@ -836,7 +939,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:15">
       <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
@@ -862,14 +965,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:15">
+      <c r="A15" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -883,7 +986,7 @@
         <v>16</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>24</v>
@@ -892,67 +995,85 @@
         <v>25</v>
       </c>
       <c r="H16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="M16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="N16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="O16" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="2" t="s">
+    <row r="17" spans="1:16" ht="25.5">
+      <c r="A17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>6</v>
+      <c r="C17" s="8">
+        <v>16593</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="2">
+        <v>47</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="1">
         <v>1234567890</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" s="1">
+        <v>2</v>
+      </c>
+      <c r="J17" s="1">
+        <v>3</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="25.5">
+      <c r="O17" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="25.5">
       <c r="A18" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="8">
         <v>16593</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -965,123 +1086,321 @@
         <v>1234567890</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I18" s="1">
+        <v>3</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L18" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="M18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1234567890</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="8" t="s">
+    <row r="22" spans="1:16">
+      <c r="A22" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="9">
+        <v>36559</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G23" s="10">
+        <v>43315</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K23" s="1">
+        <v>1111621482</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" s="9">
+        <v>39574</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G24" s="10">
+        <v>46332</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K24" s="1">
+        <v>1157972555</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="H25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K25" s="1">
+        <v>1158869930</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-    </row>
-    <row r="23" spans="1:12" ht="25.5">
-      <c r="A23" s="2" t="s">
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G30" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H30" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="I30" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="J30" s="2"/>
+      <c r="K30" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="L30" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="2" t="s">
+    <row r="31" spans="1:16">
+      <c r="A31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F31" s="2">
         <v>1234567890</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="K31" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="L31" s="1" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A22:C22"/>
+  <mergeCells count="5">
+    <mergeCell ref="A29:C29"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>